<commit_message>
Fix tests on scheduler
</commit_message>
<xml_diff>
--- a/tests/test_data/raw_mvts2.xlsx
+++ b/tests/test_data/raw_mvts2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{B2F8E6D3-0058-453C-8A39-00EB34D8D0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7B9D17D-8CE2-4A7F-A8F3-43479CBF2463}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{B2F8E6D3-0058-453C-8A39-00EB34D8D0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C868367C-1806-495E-9573-110D03CD0FEA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE849C7B-62D9-42D4-BE4C-70410574EBFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE849C7B-62D9-42D4-BE4C-70410574EBFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="69">
   <si>
     <t>Posting Date</t>
   </si>
@@ -620,19 +620,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99429E3A-888B-4DD7-A5A6-6D9C016829BE}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44930</v>
       </c>
@@ -729,7 +729,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44930</v>
       </c>
@@ -776,7 +776,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44930</v>
       </c>
@@ -823,7 +823,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44930</v>
       </c>
@@ -870,7 +870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44928</v>
       </c>
@@ -917,7 +917,7 @@
         <v>156.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44928</v>
       </c>
@@ -964,7 +964,7 @@
         <v>156.5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44928</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44928</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44928</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>156.5</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44953</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44953</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44953</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44939</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44939</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44957</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44957</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44957</v>
       </c>
@@ -1479,6 +1479,53 @@
       </c>
       <c r="P18">
         <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44928</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19">
+        <v>-0.5</v>
+      </c>
+      <c r="P19">
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>